<commit_message>
Update test results with fix
Update test results with fix
</commit_message>
<xml_diff>
--- a/createSystemData/data_tests/testResults_general_config.xlsx
+++ b/createSystemData/data_tests/testResults_general_config.xlsx
@@ -2205,8 +2205,12 @@
       <c r="G31" t="n">
         <v>0</v>
       </c>
-      <c r="H31"/>
-      <c r="I31"/>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -2230,8 +2234,12 @@
       <c r="G32" t="n">
         <v>0</v>
       </c>
-      <c r="H32"/>
-      <c r="I32"/>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding vibrio and associated tests
</commit_message>
<xml_diff>
--- a/createSystemData/data_tests/testResults_general_config.xlsx
+++ b/createSystemData/data_tests/testResults_general_config.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t xml:space="preserve">table</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t xml:space="preserve">slrImpacts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testDev</t>
   </si>
   <si>
     <t xml:space="preserve">co_sectorsRef</t>
@@ -352,8 +355,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I20" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I21" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I21"/>
   <tableColumns count="9">
     <tableColumn id="1" name="table"/>
     <tableColumn id="2" name="itemClass"/>
@@ -370,8 +373,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I31" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I32" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
     <tableColumn id="1" name="table"/>
     <tableColumn id="2" name="itemClass"/>
@@ -724,10 +727,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -782,10 +785,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>18116</v>
+        <v>18767</v>
       </c>
       <c r="E4" t="n">
-        <v>18116</v>
+        <v>18767</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -869,10 +872,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -898,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -927,10 +930,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1185,13 +1188,13 @@
         <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E18" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1214,13 +1217,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1243,24 +1246,53 @@
         <v>10</v>
       </c>
       <c r="C20" t="n">
+        <v>3</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="n">
         <v>18</v>
       </c>
-      <c r="D20" t="n">
-        <v>73</v>
-      </c>
-      <c r="E20" t="n">
-        <v>73</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" t="n">
+      <c r="D21" t="n">
+        <v>76</v>
+      </c>
+      <c r="E21" t="n">
+        <v>76</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1321,10 +1353,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -1379,10 +1411,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>18116</v>
+        <v>18767</v>
       </c>
       <c r="E4" t="n">
-        <v>18116</v>
+        <v>18767</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1466,10 +1498,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1495,10 +1527,10 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1524,10 +1556,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1782,13 +1814,13 @@
         <v>10</v>
       </c>
       <c r="C18" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E18" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1811,13 +1843,13 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1840,13 +1872,13 @@
         <v>10</v>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D20" t="n">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1869,13 +1901,13 @@
         <v>10</v>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D21" t="n">
-        <v>306</v>
+        <v>76</v>
       </c>
       <c r="E21" t="n">
-        <v>306</v>
+        <v>76</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1898,13 +1930,13 @@
         <v>10</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" t="n">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="E22" t="n">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1930,10 +1962,10 @@
         <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="E23" t="n">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1956,13 +1988,13 @@
         <v>10</v>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" t="n">
-        <v>2037</v>
+        <v>291</v>
       </c>
       <c r="E24" t="n">
-        <v>2037</v>
+        <v>291</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1985,13 +2017,13 @@
         <v>10</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="n">
-        <v>291</v>
+        <v>2037</v>
       </c>
       <c r="E25" t="n">
-        <v>291</v>
+        <v>2037</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -2014,13 +2046,13 @@
         <v>10</v>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>2037</v>
+        <v>291</v>
       </c>
       <c r="E26" t="n">
-        <v>2037</v>
+        <v>291</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -2043,13 +2075,13 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>12642</v>
+        <v>2037</v>
       </c>
       <c r="E27" t="n">
-        <v>12642</v>
+        <v>2037</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -2072,13 +2104,13 @@
         <v>10</v>
       </c>
       <c r="C28" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D28" t="n">
-        <v>30846</v>
+        <v>12642</v>
       </c>
       <c r="E28" t="n">
-        <v>30846</v>
+        <v>12642</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -2101,13 +2133,13 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>148701</v>
+        <v>30846</v>
       </c>
       <c r="E29" t="n">
-        <v>148701</v>
+        <v>30846</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -2127,16 +2159,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D30" t="n">
-        <v>2089</v>
+        <v>154812</v>
       </c>
       <c r="E30" t="n">
-        <v>1</v>
+        <v>154812</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -2153,30 +2185,59 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
+        <v>2179</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
         <v>21</v>
       </c>
-      <c r="E31" t="n">
+      <c r="E32" t="n">
         <v>20</v>
       </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="n">
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2199,68 +2260,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Mental Health sector to main FrEDI, reconfigured and rebuilt package
</commit_message>
<xml_diff>
--- a/createSystemData/data_tests/testResults_general_config.xlsx
+++ b/createSystemData/data_tests/testResults_general_config.xlsx
@@ -727,10 +727,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -756,10 +756,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>1097</v>
+        <v>1279</v>
       </c>
       <c r="E3" t="n">
-        <v>1097</v>
+        <v>1279</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -785,10 +785,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>18767</v>
+        <v>18984</v>
       </c>
       <c r="E4" t="n">
-        <v>18767</v>
+        <v>18984</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -872,10 +872,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -901,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -930,10 +930,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -959,10 +959,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1220,10 +1220,10 @@
         <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E19" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1278,10 +1278,10 @@
         <v>18</v>
       </c>
       <c r="D21" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E21" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1353,10 +1353,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -1382,10 +1382,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>1097</v>
+        <v>1279</v>
       </c>
       <c r="E3" t="n">
-        <v>1097</v>
+        <v>1279</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1411,10 +1411,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="n">
-        <v>18767</v>
+        <v>18984</v>
       </c>
       <c r="E4" t="n">
-        <v>18767</v>
+        <v>18984</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1498,10 +1498,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -1527,10 +1527,10 @@
         <v>4</v>
       </c>
       <c r="D8" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -1556,10 +1556,10 @@
         <v>14</v>
       </c>
       <c r="D9" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -1585,10 +1585,10 @@
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -1846,10 +1846,10 @@
         <v>7</v>
       </c>
       <c r="D19" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E19" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1904,10 +1904,10 @@
         <v>18</v>
       </c>
       <c r="D21" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E21" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -2136,10 +2136,10 @@
         <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>30846</v>
+        <v>32883</v>
       </c>
       <c r="E29" t="n">
-        <v>30846</v>
+        <v>32883</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -2165,10 +2165,10 @@
         <v>23</v>
       </c>
       <c r="D30" t="n">
-        <v>154812</v>
+        <v>156849</v>
       </c>
       <c r="E30" t="n">
-        <v>154812</v>
+        <v>156849</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -2194,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>2179</v>
+        <v>2221</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Updated scalars and rebuilt
Added scalars for Mental Health, reconfigured and rebuilt package
</commit_message>
<xml_diff>
--- a/createSystemData/data_tests/testResults_general_config.xlsx
+++ b/createSystemData/data_tests/testResults_general_config.xlsx
@@ -756,10 +756,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>1475</v>
+        <v>1489</v>
       </c>
       <c r="E3" t="n">
-        <v>1475</v>
+        <v>1489</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -1382,10 +1382,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>1475</v>
+        <v>1489</v>
       </c>
       <c r="E3" t="n">
-        <v>1475</v>
+        <v>1489</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>

</xml_diff>